<commit_message>
commiting new xlxs utility and Data driven login test cases files
</commit_message>
<xml_diff>
--- a/src/test/java/com/impledge/shipnauticv1/testdata/demoWorkSheet.xlsx
+++ b/src/test/java/com/impledge/shipnauticv1/testdata/demoWorkSheet.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\shipnauticv1\src\test\java\com\impledge\shipnauticv1\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\SeleniumTestProjectV1\src\test\java\com\impledge\shipnauticv1\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3396857-FE68-45C1-BA15-69AC5A1B1F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F91516-21D6-4ED5-AFC4-BBE893DE5418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>S.No.</t>
   </si>
@@ -63,10 +63,28 @@
     <t>Password1</t>
   </si>
   <si>
-    <t>amberqa@mailinator.com</t>
-  </si>
-  <si>
     <t>amitba@mailinator.com</t>
+  </si>
+  <si>
+    <t>amberroad@mailinator.com</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>amitqaMain - Admin</t>
+  </si>
+  <si>
+    <t>AmberRoad - Sub Account Admin</t>
+  </si>
+  <si>
+    <t>ParcelShipment - Sub Account Admin</t>
+  </si>
+  <si>
+    <t>Mainamitba - Admin</t>
   </si>
 </sst>
 </file>
@@ -98,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,15 +124,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -396,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,9 +441,10 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +457,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -436,8 +477,12 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -450,8 +495,12 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -459,13 +508,17 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -473,11 +526,15 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
commiting for product & contact test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/impledge/shipnauticv1/testdata/demoWorkSheet.xlsx
+++ b/src/test/java/com/impledge/shipnauticv1/testdata/demoWorkSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\SeleniumTestProjectV1\src\test\java\com\impledge\shipnauticv1\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13F09F6-7A34-4015-B17E-3E19F75C2DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB725E97-FBC2-48E6-B900-65B47A122803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>S.No.</t>
   </si>
@@ -87,7 +87,10 @@
     <t>Mainamitba - Admin</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>lccautomation@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,17 +478,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -503,9 +502,7 @@
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -523,9 +520,7 @@
       <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -543,9 +538,25 @@
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -553,8 +564,9 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F7B0D64F-913B-4A88-AE56-63D6CC24C998}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{5A131AF7-15B2-4AD9-83F7-C8E486021372}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{158ED219-89EC-471D-8CC5-36C70F1CF24C}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{24ACEDD7-5ECE-4CFB-A100-506C089414F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>